<commit_message>
Formatted power outage data
</commit_message>
<xml_diff>
--- a/Weather Data Analysis/Untouched Copy/Houston, TX/Texas.xlsx
+++ b/Weather Data Analysis/Untouched Copy/Houston, TX/Texas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhay/Desktop/powerCheck/Collected Power Outage Data DOE/Above 40 entries - Group 1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhay/Desktop/powerCheck/Weather Data Analysis/Untouched Copy/Houston, TX/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{B0B386D1-79D5-8F43-8D57-E6303B6CF2A5}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{3F522D35-AA41-AF4F-8C54-ECAB96089AF1}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="300" yWindow="460" windowWidth="28040" windowHeight="15700" xr2:uid="{6A4BE853-6BA8-894D-B13D-7CBDB9EAD733}"/>
   </bookViews>

</xml_diff>